<commit_message>
20191216{the practical/Oral Exam_3 }
</commit_message>
<xml_diff>
--- a/Projects/DSS/What If/WhatIf.xlsx
+++ b/Projects/DSS/What If/WhatIf.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CISISDEPARTMENT\4th_Grade_IS-Master-\Projects\DSS\What If\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9788A0-1825-48E6-8A00-E385E645037E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50263554-DD3F-4FF1-9678-FA6BED39A575}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1008" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t xml:space="preserve">price </t>
   </si>
@@ -70,6 +70,12 @@
       </rPr>
       <t>t</t>
     </r>
+  </si>
+  <si>
+    <t>discount</t>
+  </si>
+  <si>
+    <t>NetPrice</t>
   </si>
 </sst>
 </file>
@@ -174,25 +180,26 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="2" fillId="2" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="60% - Accent1" xfId="5" builtinId="32"/>
@@ -478,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:J27"/>
+  <dimension ref="A2:T27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A27"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,45 +496,64 @@
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
     <col min="2" max="6" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="M4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" s="10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="25.8" x14ac:dyDescent="0.5">
       <c r="C6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -559,9 +585,31 @@
       <c r="J7" s="4">
         <v>200</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="M7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N7" s="1">
+        <f>N2*N3*(1-N4)</f>
+        <v>5600</v>
+      </c>
+      <c r="O7">
+        <v>25</v>
+      </c>
+      <c r="P7">
+        <v>30</v>
+      </c>
+      <c r="Q7">
+        <v>35</v>
+      </c>
+      <c r="R7">
+        <v>40</v>
+      </c>
+      <c r="S7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="5">
@@ -592,9 +640,31 @@
       <c r="J8" s="1">
         <v>900</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
+      <c r="N8">
+        <v>5</v>
+      </c>
+      <c r="O8">
+        <f t="dataTable" ref="O8:T15" dt2D="1" dtr="1" r1="N2" r2="N3"/>
+        <v>100</v>
+      </c>
+      <c r="P8">
+        <v>120</v>
+      </c>
+      <c r="Q8">
+        <v>140</v>
+      </c>
+      <c r="R8">
+        <v>160</v>
+      </c>
+      <c r="S8">
+        <v>180</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" s="7"/>
       <c r="B9" s="5">
         <v>10</v>
       </c>
@@ -622,9 +692,30 @@
       <c r="J9" s="1">
         <v>1800</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
+      <c r="N9">
+        <v>10</v>
+      </c>
+      <c r="O9">
+        <v>200</v>
+      </c>
+      <c r="P9">
+        <v>240</v>
+      </c>
+      <c r="Q9">
+        <v>280</v>
+      </c>
+      <c r="R9">
+        <v>320</v>
+      </c>
+      <c r="S9">
+        <v>360</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
       <c r="B10" s="5">
         <v>15</v>
       </c>
@@ -652,9 +743,30 @@
       <c r="J10" s="1">
         <v>2700</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
+      <c r="N10">
+        <v>15</v>
+      </c>
+      <c r="O10">
+        <v>300</v>
+      </c>
+      <c r="P10">
+        <v>360</v>
+      </c>
+      <c r="Q10">
+        <v>420</v>
+      </c>
+      <c r="R10">
+        <v>480</v>
+      </c>
+      <c r="S10">
+        <v>540</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
       <c r="B11" s="5">
         <v>20</v>
       </c>
@@ -682,9 +794,30 @@
       <c r="J11" s="1">
         <v>3600</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
+      <c r="N11">
+        <v>20</v>
+      </c>
+      <c r="O11">
+        <v>400</v>
+      </c>
+      <c r="P11">
+        <v>480</v>
+      </c>
+      <c r="Q11">
+        <v>560</v>
+      </c>
+      <c r="R11">
+        <v>640</v>
+      </c>
+      <c r="S11">
+        <v>720</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12" s="7"/>
       <c r="B12" s="5">
         <v>25</v>
       </c>
@@ -712,9 +845,30 @@
       <c r="J12" s="1">
         <v>4500</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
+      <c r="N12">
+        <v>25</v>
+      </c>
+      <c r="O12">
+        <v>500</v>
+      </c>
+      <c r="P12">
+        <v>600</v>
+      </c>
+      <c r="Q12">
+        <v>700</v>
+      </c>
+      <c r="R12">
+        <v>800</v>
+      </c>
+      <c r="S12">
+        <v>900</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" s="7"/>
       <c r="B13" s="5">
         <v>30</v>
       </c>
@@ -742,9 +896,30 @@
       <c r="J13" s="1">
         <v>5400</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
+      <c r="N13">
+        <v>30</v>
+      </c>
+      <c r="O13">
+        <v>600</v>
+      </c>
+      <c r="P13">
+        <v>720</v>
+      </c>
+      <c r="Q13">
+        <v>840</v>
+      </c>
+      <c r="R13">
+        <v>960</v>
+      </c>
+      <c r="S13">
+        <v>1080</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14" s="7"/>
       <c r="B14" s="5">
         <v>35</v>
       </c>
@@ -772,9 +947,30 @@
       <c r="J14" s="1">
         <v>6300</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
+      <c r="N14">
+        <v>35</v>
+      </c>
+      <c r="O14">
+        <v>700</v>
+      </c>
+      <c r="P14">
+        <v>840</v>
+      </c>
+      <c r="Q14">
+        <v>980</v>
+      </c>
+      <c r="R14">
+        <v>1120</v>
+      </c>
+      <c r="S14">
+        <v>1260</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15" s="7"/>
       <c r="B15" s="5">
         <v>40</v>
       </c>
@@ -802,9 +998,30 @@
       <c r="J15" s="1">
         <v>7200</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
+      <c r="N15">
+        <v>40</v>
+      </c>
+      <c r="O15">
+        <v>800</v>
+      </c>
+      <c r="P15">
+        <v>960</v>
+      </c>
+      <c r="Q15">
+        <v>1120</v>
+      </c>
+      <c r="R15">
+        <v>1280</v>
+      </c>
+      <c r="S15">
+        <v>1440</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16" s="7"/>
       <c r="B16" s="5">
         <v>45</v>
       </c>
@@ -834,7 +1051,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
+      <c r="A17" s="7"/>
       <c r="B17" s="5">
         <v>50</v>
       </c>
@@ -864,7 +1081,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
+      <c r="A18" s="7"/>
       <c r="B18" s="5">
         <v>55</v>
       </c>
@@ -894,7 +1111,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
+      <c r="A19" s="7"/>
       <c r="B19" s="5">
         <v>60</v>
       </c>
@@ -924,7 +1141,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
+      <c r="A20" s="7"/>
       <c r="B20" s="5">
         <v>65</v>
       </c>
@@ -954,7 +1171,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
+      <c r="A21" s="7"/>
       <c r="B21" s="5">
         <v>70</v>
       </c>
@@ -984,7 +1201,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="6"/>
+      <c r="A22" s="7"/>
       <c r="B22" s="5">
         <v>75</v>
       </c>
@@ -1014,7 +1231,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
+      <c r="A23" s="7"/>
       <c r="B23" s="5">
         <v>80</v>
       </c>
@@ -1044,7 +1261,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="6"/>
+      <c r="A24" s="7"/>
       <c r="B24" s="5">
         <v>85</v>
       </c>
@@ -1074,7 +1291,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="6"/>
+      <c r="A25" s="7"/>
       <c r="B25" s="5">
         <v>90</v>
       </c>
@@ -1104,7 +1321,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="6"/>
+      <c r="A26" s="7"/>
       <c r="B26" s="5">
         <v>95</v>
       </c>
@@ -1134,7 +1351,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="6"/>
+      <c r="A27" s="7"/>
       <c r="B27" s="5">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
20200309{Add Week 4 resources _1}
</commit_message>
<xml_diff>
--- a/Projects/DSS/What If/WhatIf.xlsx
+++ b/Projects/DSS/What If/WhatIf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CISISDEPARTMENT\4th_Grade_IS-Master-\Projects\DSS\What If\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50263554-DD3F-4FF1-9678-FA6BED39A575}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9B5C6E-FB84-430A-8033-8FB785F9C494}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1008" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -180,13 +180,14 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="2" fillId="2" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="4"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -199,7 +200,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="60% - Accent1" xfId="5" builtinId="32"/>
@@ -485,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:T27"/>
+  <dimension ref="A2:T34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="B7" sqref="B7:J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,21 +538,21 @@
       <c r="M4" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="10">
+      <c r="N4" s="6">
         <v>0.2</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -609,7 +610,7 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="5">
@@ -664,7 +665,7 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="5">
         <v>10</v>
       </c>
@@ -715,7 +716,7 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="5">
         <v>15</v>
       </c>
@@ -766,7 +767,7 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="5">
         <v>20</v>
       </c>
@@ -817,7 +818,7 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="5">
         <v>25</v>
       </c>
@@ -868,7 +869,7 @@
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="5">
         <v>30</v>
       </c>
@@ -919,7 +920,7 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="5">
         <v>35</v>
       </c>
@@ -970,7 +971,7 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
+      <c r="A15" s="8"/>
       <c r="B15" s="5">
         <v>40</v>
       </c>
@@ -1021,7 +1022,7 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="5">
         <v>45</v>
       </c>
@@ -1049,9 +1050,13 @@
       <c r="J16" s="1">
         <v>8100</v>
       </c>
+      <c r="M16" s="11">
+        <f>0.8*125</f>
+        <v>100</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
+      <c r="A17" s="8"/>
       <c r="B17" s="5">
         <v>50</v>
       </c>
@@ -1081,7 +1086,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
+      <c r="A18" s="8"/>
       <c r="B18" s="5">
         <v>55</v>
       </c>
@@ -1111,7 +1116,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
+      <c r="A19" s="8"/>
       <c r="B19" s="5">
         <v>60</v>
       </c>
@@ -1141,7 +1146,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
+      <c r="A20" s="8"/>
       <c r="B20" s="5">
         <v>65</v>
       </c>
@@ -1171,7 +1176,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
+      <c r="A21" s="8"/>
       <c r="B21" s="5">
         <v>70</v>
       </c>
@@ -1201,7 +1206,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
+      <c r="A22" s="8"/>
       <c r="B22" s="5">
         <v>75</v>
       </c>
@@ -1231,7 +1236,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="7"/>
+      <c r="A23" s="8"/>
       <c r="B23" s="5">
         <v>80</v>
       </c>
@@ -1261,7 +1266,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
+      <c r="A24" s="8"/>
       <c r="B24" s="5">
         <v>85</v>
       </c>
@@ -1291,7 +1296,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="7"/>
+      <c r="A25" s="8"/>
       <c r="B25" s="5">
         <v>90</v>
       </c>
@@ -1321,7 +1326,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
+      <c r="A26" s="8"/>
       <c r="B26" s="5">
         <v>95</v>
       </c>
@@ -1351,7 +1356,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
+      <c r="A27" s="8"/>
       <c r="B27" s="5">
         <v>100</v>
       </c>
@@ -1378,6 +1383,11 @@
       </c>
       <c r="J27" s="1">
         <v>18000</v>
+      </c>
+    </row>
+    <row r="34" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O34">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>